<commit_message>
I have updated lead_scraper.py to prompt for the output file name before scraping begins. The scraping process is now wrapped in a finally block, ensuring that any collected data is   automatically saved even if the script crashes or is manually interrupted
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,18 +596,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Peace Innovative Real Estate Ltd. (@peaceinnovative. ...</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+          <t>Modern Letter R Real Estate Logo</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>+1(215)796-4570</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/peaceinnovative.realestate/</t>
+          <t>https://www.instagram.com/p/DPb03GeEgJK/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>peaceinnovative.realestate@gmail.com</t>
+          <t>professionallogolads@gmail.com</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -620,18 +624,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Luxurious Apartment For Sale in Uttora (Sector 4, Road#6/ ...</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+          <t>Modern Luxury Interior Project At Bashundhara R/A + ...</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0140339995</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/p/CwAWoIMp3J9/</t>
+          <t>https://www.instagram.com/reel/DTFRT_FAeoA/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>careers.studiodhakaltd@gmail.com</t>
+          <t>premiumtouchdecor@gmail.com</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -668,18 +676,18 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>📢 Internship Opportunity – Night Shift (US Real Estate) ...</t>
+          <t>Peace Innovative Real Estate Ltd. (@peaceinnovative. ...</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/p/DTB849qk3PP/</t>
+          <t>https://www.instagram.com/peaceinnovative.realestate/</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>bscgroupbd@gmail.com</t>
+          <t>peaceinnovative.realestate@gmail.com</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -692,18 +700,18 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>: Modern Flat for Sale in Dhaka! Looking for your dream home ...</t>
+          <t>Luxurious Apartment For Sale in Uttora (Sector 4, Road#6/ ...</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/reel/DUdpRqKjpy8/</t>
+          <t>https://www.instagram.com/p/CwAWoIMp3J9/</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>dproperty.com.bd@gmail.com</t>
+          <t>careers.studiodhakaltd@gmail.com</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -716,18 +724,18 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>New Launch Luxury Apartments! "REGEYA VILLA ...</t>
+          <t>AIM Properties — Professional. Personal. Reliable. Finding ...</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/p/DNd3kpSg4Yl/</t>
+          <t>https://www.instagram.com/p/DR4FoafjWrz/</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>structureshine@gmail.com</t>
+          <t>pmgroupebd@gmail.comread</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -740,18 +748,18 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AIM Properties — Professional. Personal. Reliable. Finding ...</t>
+          <t>ঢাকা ওয়েস্টার্ন ভ্যালি প্রকল্প এলাকায় নির্মাণ কাজ ...</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/p/DR4FoafjWrz/</t>
+          <t>https://www.instagram.com/reel/DTpyYe0DYBu/</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>pmgroupebd@gmail.comread</t>
+          <t>info.faithrealestate@gmail.com</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -764,18 +772,18 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ঢাকা ওয়েস্টার্ন ভ্যালি প্রকল্প এলাকায় নির্মাণ কাজ ...</t>
+          <t>Luxury Living Redefined in Baridhara! 🏢✨🇧🇩 Concord ...</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/reel/DTpyYe0DYBu/</t>
+          <t>https://www.instagram.com/p/DTvlM5xlV-m/</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>info.faithrealestate@gmail.com</t>
+          <t>pmgroupebd@gmail.com</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -788,18 +796,18 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Luxury Living Redefined in Baridhara! 🏢✨🇧🇩 Concord ...</t>
+          <t>Project : Troyee Number of Floors : G + 7 Living Floors Ground ...</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/p/DTvlM5xlV-m/</t>
+          <t>https://www.instagram.com/reel/DUAqnqeglpd/</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>pmgroupebd@gmail.com</t>
+          <t>greenhutshafin@gmail.com</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -812,18 +820,18 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Project : Troyee Number of Floors : G + 7 Living Floors Ground ...</t>
+          <t>#broucer</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/reel/DUAqnqeglpd/</t>
+          <t>https://www.instagram.com/p/DU0joeKCB5x/</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>greenhutshafin@gmail.com</t>
+          <t>graphicsdac@gmail.com</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -836,18 +844,18 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>#broucer</t>
+          <t>📢 Internship Opportunity – Night Shift (US Real Estate) ...</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/p/DU0joeKCB5x/</t>
+          <t>https://www.instagram.com/p/DTB849qk3PP/</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>graphicsdac@gmail.com</t>
+          <t>bscgroupbd@gmail.com</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -860,18 +868,18 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>At REHAB Fair, Navana Real Estate presents a refined ...</t>
+          <t>: Modern Flat for Sale in Dhaka! Looking for your dream home ...</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/reel/DSkJHTmkmqn/</t>
+          <t>https://www.instagram.com/reel/DUdpRqKjpy8/</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>arushrealtor@gmail.com</t>
+          <t>dproperty.com.bd@gmail.com</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -884,18 +892,18 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Pixles Lab (@pixles_lab) · Dhaka, Bangladesh</t>
+          <t>New Launch Luxury Apartments! "REGEYA VILLA ...</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/pixles_lab/</t>
+          <t>https://www.instagram.com/p/DNd3kpSg4Yl/</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>thepixleslab@gmail.com</t>
+          <t>structureshine@gmail.com</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -908,16 +916,20 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Anam &amp; Naher Real Estate Ltd.(ANREL) (@anamnaher. ...</t>
+          <t>House No 59/A, Road No: 12/A, Dhanmondi, DHaka-1209. ...</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/anamnaher.realestate/</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
+          <t>https://www.instagram.com/p/CegXiQNv1A0/</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>studiodhakatld@gmail.com</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
           <t>Google Search</t>
@@ -928,16 +940,20 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Notun Thikana (@notunthikana22) · Dhaka</t>
+          <t>Pixles Lab (@pixles_lab) · Dhaka, Bangladesh</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/notunthikana22/</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
+          <t>https://www.instagram.com/pixles_lab/</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>thepixleslab@gmail.com</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
           <t>Google Search</t>
@@ -948,16 +964,20 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Purbachal Estate Agency (@estateagency.com.bd)</t>
+          <t>At REHAB Fair, Navana Real Estate presents a refined ...</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/estateagency.com.bd/</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
+          <t>https://www.instagram.com/reel/DSkJHTmkmqn/</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>arushrealtor@gmail.com</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr">
         <is>
           <t>Google Search</t>
@@ -968,22 +988,226 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Maruf Raihan.Works (@marufraihan.works)</t>
+          <t>Ariyan Islam Rifat (@_mr.ariyan)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
+          <t>https://www.instagram.com/_mr.ariyan/</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>mr.ariyanislam2500@gmail.com</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Welcome to JBS Gazi Landmark, a premium residential ...</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DTrnUR8D0Cq/</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>jsbuildersltdofficial@gmail.com</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>️ বাড়ি নির্মাণের আগে অবহেলা নয়— সঠিক সিদ্ধান্তই নিরাপদ ...</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DUkYO8ukeii/</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>pisconsultantfimbd@gmail.com</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>🚧 Dhaka Western Valley Project – উন্নয়নের পথে আরও এক ধাপ ...</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DTe3e4rAcAP/</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>dhakawesternvalley@gmail.com</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Real Estate Logo Design</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/C9k00kVyee3/?img_index=5</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>nusratnahianr@gmail.com</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>IS THIS REALLY DHAKA? You have to see it to believe it!!</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DNqUDx502F-/</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>snowwspaces@gmail.com</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Anam &amp; Naher Real Estate Ltd.(ANREL) (@anamnaher. ...</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/anamnaher.realestate/</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Notun Thikana (@notunthikana22) · Dhaka</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/notunthikana22/</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Purbachal Estate Agency (@estateagency.com.bd)</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/estateagency.com.bd/</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Maruf Raihan.Works (@marufraihan.works)</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>https://www-fallback.instagram.com/marufraihan.works/</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Google Search</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Google Search</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>